<commit_message>
added instructions for distraction
</commit_message>
<xml_diff>
--- a/01_Paradigms/ER-ED/ER_Training/blocks_training.xlsx
+++ b/01_Paradigms/ER-ED/ER_Training/blocks_training.xlsx
@@ -119,7 +119,7 @@
     <t>Dieses Mal sollen Sie die Position eines uninvolvierten Beobachters einnehmen. Denken Sie über das Bild in einer neutralen Weise nach.</t>
   </si>
   <si>
-    <t>DAS HIER IST NUR EIN PLATZHALTER</t>
+    <t>Denken Sie während des Betrachtens der Bilder an etwas Neutrales, das mit dem Bild nichts zu tun hat. Das könnten geometrische Figuren, Alltagstätigkeiten oder bekannte Orte sein.</t>
   </si>
 </sst>
 </file>
@@ -450,7 +450,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>